<commit_message>
Edited 5.2.1, made an Addition for 5.2.1
</commit_message>
<xml_diff>
--- a/5.2.1/Data.xlsx
+++ b/5.2.1/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
   <si>
     <t>Динамический метод</t>
   </si>
@@ -45,10 +45,13 @@
     <t>Va, В</t>
   </si>
   <si>
-    <t>Iк, мА</t>
+    <t>Iк, мкА</t>
   </si>
   <si>
-    <t>Iк, мкА</t>
+    <t>I0, мкА</t>
+  </si>
+  <si>
+    <t>I~, мкА</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49:J57"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F74" sqref="E74:F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -595,17 +598,35 @@
       <c r="B19" t="s">
         <v>9</v>
       </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
         <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
       </c>
       <c r="I19" t="s">
         <v>8</v>
       </c>
       <c r="J19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
         <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -613,11 +634,15 @@
         <v>2.95</v>
       </c>
       <c r="B20">
-        <v>2.8000000000000001E-2</v>
+        <v>28</v>
       </c>
       <c r="C20">
-        <f>B20 * 1000</f>
-        <v>28</v>
+        <f>12.5321106194744 + 6.40918573732954 * A20 - 0.105645947480177 * A20*A20 + 0.00172074354709666*A20*A20*A20  - 1.22543389562474 * A20*A20*A20*A20 / 100000</f>
+        <v>30.563072196214268</v>
+      </c>
+      <c r="D20">
+        <f>B20-C20</f>
+        <v>-2.563072196214268</v>
       </c>
       <c r="E20">
         <v>2.35</v>
@@ -637,11 +662,15 @@
         <v>3.65</v>
       </c>
       <c r="B21">
-        <v>3.2000000000000001E-2</v>
+        <v>32</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:C65" si="0">B21 * 1000</f>
-        <v>32</v>
+        <f t="shared" ref="C21:C65" si="0">12.5321106194744 + 6.40918573732954 * A21 - 0.105645947480177 * A21*A21 + 0.00172074354709666*A21*A21*A21  - 1.22543389562474 * A21*A21*A21*A21 / 100000</f>
+        <v>34.599670226536588</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D65" si="1">B21-C21</f>
+        <v>-2.5996702265365883</v>
       </c>
       <c r="E21">
         <v>4.22</v>
@@ -661,11 +690,15 @@
         <v>4.55</v>
       </c>
       <c r="B22">
-        <v>3.7999999999999999E-2</v>
+        <v>38</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>39.663606170956555</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>-1.6636061709565553</v>
       </c>
       <c r="E22">
         <v>5.76</v>
@@ -685,11 +718,15 @@
         <v>6.33</v>
       </c>
       <c r="B23">
-        <v>5.2999999999999999E-2</v>
+        <v>53</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>49.285907631414958</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>3.7140923685850424</v>
       </c>
       <c r="E23">
         <v>6.44</v>
@@ -709,11 +746,15 @@
         <v>7.18</v>
       </c>
       <c r="B24">
-        <v>0.06</v>
+        <v>60</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>53.708121067557165</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>6.2918789324428346</v>
       </c>
       <c r="E24">
         <v>8.58</v>
@@ -733,11 +774,15 @@
         <v>8.24</v>
       </c>
       <c r="B25">
-        <v>6.8000000000000005E-2</v>
+        <v>68</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>59.076916380638039</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>8.9230836193619609</v>
       </c>
       <c r="E25">
         <v>9.7100000000000009</v>
@@ -757,11 +802,15 @@
         <v>9.94</v>
       </c>
       <c r="B26">
-        <v>8.1000000000000003E-2</v>
+        <v>81</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>67.371543832082537</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>13.628456167917463</v>
       </c>
       <c r="E26">
         <v>11.42</v>
@@ -781,11 +830,15 @@
         <v>11.37</v>
       </c>
       <c r="B27">
-        <v>9.0999999999999998E-2</v>
+        <v>91</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>74.071454709471752</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>16.928545290528248</v>
       </c>
       <c r="E27">
         <v>13.88</v>
@@ -805,11 +858,15 @@
         <v>13.52</v>
       </c>
       <c r="B28">
-        <v>0.107</v>
+        <v>107</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>83.716309393867675</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>23.283690606132325</v>
       </c>
       <c r="E28">
         <v>16.02</v>
@@ -829,11 +886,15 @@
         <v>15.17</v>
       </c>
       <c r="B29">
-        <v>0.11799999999999999</v>
+        <v>118</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>90.805502303001248</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>27.194497696998752</v>
       </c>
       <c r="E29">
         <v>17.61</v>
@@ -853,11 +914,15 @@
         <v>16.61</v>
       </c>
       <c r="B30">
-        <v>0.128</v>
+        <v>128</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>128</v>
+        <v>96.794470559241674</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>31.205529440758326</v>
       </c>
       <c r="E30">
         <v>19.34</v>
@@ -877,11 +942,15 @@
         <v>18.05</v>
       </c>
       <c r="B31">
-        <v>0.13700000000000001</v>
+        <v>137</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>102.61667177920809</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>34.38332822079191</v>
       </c>
       <c r="E31">
         <v>19.97</v>
@@ -901,11 +970,15 @@
         <v>18.77</v>
       </c>
       <c r="B32">
-        <v>0.14099999999999999</v>
+        <v>141</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>141</v>
+        <v>105.47016216107609</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>35.52983783892391</v>
       </c>
       <c r="E32">
         <v>20.62</v>
@@ -925,11 +998,15 @@
         <v>19.829999999999998</v>
       </c>
       <c r="B33">
-        <v>0.14199999999999999</v>
+        <v>142</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>142</v>
+        <v>109.60624029827738</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>32.393759701722615</v>
       </c>
       <c r="E33">
         <v>21.31</v>
@@ -949,11 +1026,15 @@
         <v>20.420000000000002</v>
       </c>
       <c r="B34">
-        <v>0.14000000000000001</v>
+        <v>140</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>111.87670592274371</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>28.12329407725629</v>
       </c>
       <c r="E34">
         <v>22.67</v>
@@ -973,11 +1054,15 @@
         <v>20.82</v>
       </c>
       <c r="B35">
-        <v>0.13700000000000001</v>
+        <v>137</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>113.4037160121499</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>23.5962839878501</v>
       </c>
       <c r="E35">
         <v>23.3</v>
@@ -997,11 +1082,15 @@
         <v>21.53</v>
       </c>
       <c r="B36">
-        <v>0.13100000000000001</v>
+        <v>131</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>116.0906519413673</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>14.909348058632702</v>
       </c>
       <c r="E36">
         <v>23.79</v>
@@ -1021,11 +1110,15 @@
         <v>22.14</v>
       </c>
       <c r="B37">
-        <v>0.123</v>
+        <v>123</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>118.37607123944416</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>4.6239287605558417</v>
       </c>
       <c r="E37">
         <v>24.24</v>
@@ -1045,11 +1138,15 @@
         <v>23.01</v>
       </c>
       <c r="B38">
-        <v>7.6999999999999999E-2</v>
+        <v>77</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>121.60053303025337</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>-44.600533030253374</v>
       </c>
       <c r="E38">
         <v>25.08</v>
@@ -1069,11 +1166,15 @@
         <v>23.61</v>
       </c>
       <c r="B39">
-        <v>6.5000000000000002E-2</v>
+        <v>65</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>123.80140351911456</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>-58.801403519114558</v>
       </c>
       <c r="E39">
         <v>25.62</v>
@@ -1093,11 +1194,15 @@
         <v>24.81</v>
       </c>
       <c r="B40">
-        <v>6.7000000000000004E-2</v>
+        <v>67</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>128.1503829936394</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>-61.150382993639397</v>
       </c>
       <c r="E40">
         <v>27.82</v>
@@ -1117,11 +1222,15 @@
         <v>26.38</v>
       </c>
       <c r="B41">
-        <v>8.6999999999999994E-2</v>
+        <v>87</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>133.74172134364969</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>-46.741721343649687</v>
       </c>
       <c r="E41">
         <v>29.46</v>
@@ -1141,11 +1250,15 @@
         <v>27.82</v>
       </c>
       <c r="B42">
-        <v>0.108</v>
+        <v>108</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>138.78028729365056</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>-30.780287293650559</v>
       </c>
       <c r="E42">
         <v>30.66</v>
@@ -1165,11 +1278,15 @@
         <v>28.77</v>
       </c>
       <c r="B43">
-        <v>0.121</v>
+        <v>121</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>142.06089970375788</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>-21.060899703757883</v>
       </c>
       <c r="E43">
         <v>32.06</v>
@@ -1189,11 +1306,15 @@
         <v>29.56</v>
       </c>
       <c r="B44">
-        <v>0.13100000000000001</v>
+        <v>131</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>144.76418159627693</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>-13.764181596276927</v>
       </c>
       <c r="E44">
         <v>33.96</v>
@@ -1213,11 +1334,15 @@
         <v>30.66</v>
       </c>
       <c r="B45">
-        <v>0.14499999999999999</v>
+        <v>145</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>148.49243513267615</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>-3.4924351326761496</v>
       </c>
       <c r="E45">
         <v>35.29</v>
@@ -1237,11 +1362,15 @@
         <v>31.25</v>
       </c>
       <c r="B46">
-        <v>0.153</v>
+        <v>153</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>150.47557162941439</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>2.5244283705856105</v>
       </c>
       <c r="E46">
         <v>37.06</v>
@@ -1261,11 +1390,15 @@
         <v>32.58</v>
       </c>
       <c r="B47">
-        <v>0.16800000000000001</v>
+        <v>168</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>154.90516019788149</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>13.094839802118514</v>
       </c>
       <c r="E47">
         <v>38.42</v>
@@ -1285,11 +1418,15 @@
         <v>32.74</v>
       </c>
       <c r="B48">
-        <v>0.17100000000000001</v>
+        <v>171</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>171</v>
+        <v>155.43430746445546</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>15.565692535544542</v>
       </c>
       <c r="E48">
         <v>39.33</v>
@@ -1309,11 +1446,15 @@
         <v>34.119999999999997</v>
       </c>
       <c r="B49">
-        <v>0.187</v>
+        <v>187</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>187</v>
+        <v>159.96562936019137</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>27.034370639808628</v>
       </c>
       <c r="E49">
         <v>41.96</v>
@@ -1333,11 +1474,15 @@
         <v>35.54</v>
       </c>
       <c r="B50">
-        <v>0.2</v>
+        <v>200</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>164.5681375701094</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>35.4318624298906</v>
       </c>
       <c r="E50">
         <v>44.39</v>
@@ -1357,11 +1502,15 @@
         <v>36.29</v>
       </c>
       <c r="B51">
-        <v>0.20200000000000001</v>
+        <v>202</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>202</v>
+        <v>166.97453835952109</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>35.025461640478909</v>
       </c>
       <c r="E51">
         <v>46.13</v>
@@ -1381,11 +1530,15 @@
         <v>37.18</v>
       </c>
       <c r="B52">
-        <v>0.20100000000000001</v>
+        <v>201</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>201</v>
+        <v>169.80801183069752</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>31.191988169302476</v>
       </c>
       <c r="E52">
         <v>47.8</v>
@@ -1405,11 +1558,15 @@
         <v>37.83</v>
       </c>
       <c r="B53">
-        <v>0.20100000000000001</v>
+        <v>201</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>201</v>
+        <v>171.86205074838708</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>29.137949251612923</v>
       </c>
       <c r="E53">
         <v>50.67</v>
@@ -1429,11 +1586,15 @@
         <v>40.18</v>
       </c>
       <c r="B54">
-        <v>0.187</v>
+        <v>187</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>187</v>
+        <v>179.17635202552535</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>7.8236479744746532</v>
       </c>
       <c r="E54">
         <v>52.09</v>
@@ -1453,11 +1614,15 @@
         <v>41.86</v>
       </c>
       <c r="B55">
-        <v>0.17399999999999999</v>
+        <v>174</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>174</v>
+        <v>184.29143788883613</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>-10.291437888836128</v>
       </c>
       <c r="E55">
         <v>54.54</v>
@@ -1477,11 +1642,15 @@
         <v>42.85</v>
       </c>
       <c r="B56">
-        <v>0.16900000000000001</v>
+        <v>169</v>
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>169</v>
+        <v>187.25760484226274</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>-18.257604842262737</v>
       </c>
       <c r="E56">
         <v>57.86</v>
@@ -1501,11 +1670,15 @@
         <v>46.87</v>
       </c>
       <c r="B57">
-        <v>0.16300000000000001</v>
+        <v>163</v>
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>163</v>
+        <v>198.88395426815148</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>-35.883954268151484</v>
       </c>
       <c r="E57">
         <v>60.02</v>
@@ -1525,11 +1698,15 @@
         <v>49.91</v>
       </c>
       <c r="B58">
-        <v>0.17499999999999999</v>
+        <v>175</v>
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>207.14353046625649</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>-32.143530466256493</v>
       </c>
       <c r="E58">
         <v>62.91</v>
@@ -1543,11 +1720,15 @@
         <v>52.67</v>
       </c>
       <c r="B59">
-        <v>0.192</v>
+        <v>192</v>
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>214.14525112842259</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>-22.145251128422586</v>
       </c>
       <c r="E59">
         <v>66.209999999999994</v>
@@ -1561,11 +1742,15 @@
         <v>56.51</v>
       </c>
       <c r="B60">
-        <v>0.219</v>
+        <v>219</v>
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>219</v>
+        <v>222.90352957280641</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>-3.9035295728064057</v>
       </c>
       <c r="E60">
         <v>72.19</v>
@@ -1579,11 +1764,15 @@
         <v>59.09</v>
       </c>
       <c r="B61">
-        <v>0.23100000000000001</v>
+        <v>231</v>
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>228.00050304390629</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>2.9994969560937079</v>
       </c>
       <c r="E61">
         <v>77.989999999999995</v>
@@ -1597,11 +1786,15 @@
         <v>62.12</v>
       </c>
       <c r="B62">
-        <v>0.23699999999999999</v>
+        <v>237</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>237</v>
+        <v>233.00121709845121</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>3.9987829015487932</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -1609,11 +1802,15 @@
         <v>70.86</v>
       </c>
       <c r="B63">
-        <v>0.24</v>
+        <v>240</v>
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>239.50652316886311</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>0.49347683113688845</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -1621,27 +1818,178 @@
         <v>73.849999999999994</v>
       </c>
       <c r="B64">
-        <v>0.248</v>
+        <v>248</v>
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>248</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>238.23588610801744</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>9.7641138919825607</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>78.03</v>
       </c>
       <c r="B65">
-        <v>0.26100000000000001</v>
+        <v>261</v>
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>261</v>
+        <v>232.62799171374144</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>28.372008286258563</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" t="s">
+        <v>10</v>
+      </c>
+      <c r="I69" t="s">
+        <v>8</v>
+      </c>
+      <c r="J69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70">
+        <v>2.95</v>
+      </c>
+      <c r="B70">
+        <v>28</v>
+      </c>
+      <c r="E70">
+        <v>2.35</v>
+      </c>
+      <c r="F70">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71">
+        <v>3.65</v>
+      </c>
+      <c r="B71">
+        <v>32</v>
+      </c>
+      <c r="E71">
+        <v>4.22</v>
+      </c>
+      <c r="F71">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72">
+        <v>4.55</v>
+      </c>
+      <c r="B72">
+        <v>38</v>
+      </c>
+      <c r="E72">
+        <v>5.76</v>
+      </c>
+      <c r="F72">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73">
+        <v>6.33</v>
+      </c>
+      <c r="B73">
+        <v>53</v>
+      </c>
+      <c r="E73">
+        <v>6.44</v>
+      </c>
+      <c r="F73">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74">
+        <v>7.18</v>
+      </c>
+      <c r="B74">
+        <v>60</v>
+      </c>
+      <c r="E74">
+        <v>23.3</v>
+      </c>
+      <c r="F74">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75">
+        <v>22.5</v>
+      </c>
+      <c r="B75">
+        <v>100</v>
+      </c>
+      <c r="E75">
+        <v>30.8</v>
+      </c>
+      <c r="F75">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76">
+        <v>30.66</v>
+      </c>
+      <c r="B76">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77">
+        <v>40.18</v>
+      </c>
+      <c r="B77">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78">
+        <v>56.51</v>
+      </c>
+      <c r="B78">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79">
+        <v>68</v>
+      </c>
+      <c r="B79">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:J6"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -1649,13 +1997,6 @@
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="I18:L18"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>